<commit_message>
Correcting typo in command lines
</commit_message>
<xml_diff>
--- a/e2eTesting/TestCalc.xlsx
+++ b/e2eTesting/TestCalc.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregscullard/dev/github.com/hashgraph/hedera-stable-coin-demo/e2eTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB99C17-A123-B943-A4DB-B404F50C0C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF243DE5-5318-9349-AAB2-AEAD54F59F30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53240" yWindow="1720" windowWidth="34360" windowHeight="16940" xr2:uid="{DC4929BB-FF3C-9849-AB1F-44F8695434D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -780,20 +780,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -802,23 +790,56 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -826,32 +847,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1189,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77B8886-384E-0148-B7DB-2533F7AC3104}">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="3" spans="1:21" ht="17" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="5">
@@ -1248,10 +1248,10 @@
       <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="40">
         <v>10</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="11">
         <v>10</v>
       </c>
@@ -1261,10 +1261,10 @@
       <c r="B6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="50">
+      <c r="C6" s="42">
         <v>33000</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="12">
         <v>518400</v>
       </c>
@@ -1274,10 +1274,10 @@
       <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="44">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="12">
         <v>50</v>
       </c>
@@ -1287,13 +1287,13 @@
       <c r="B8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="46">
         <f>E9/C9</f>
         <v>98.181818181818187</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="37" t="s">
+      <c r="D8" s="47"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="33" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         <f>F9*10</f>
         <v>264480000</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="33" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
         <f>D13/60</f>
         <v>24.488888888888887</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="33" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1418,196 +1418,196 @@
     </row>
     <row r="16" spans="1:21" ht="17" thickBot="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="46" t="str">
+      <c r="C16" s="53" t="str">
         <f>_xlfn.CONCAT("java -jar runme.jar ",C9)</f>
         <v>java -jar runme.jar 264000</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="46"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="46"/>
-      <c r="R16" s="46"/>
-      <c r="S16" s="46"/>
-      <c r="T16" s="46"/>
-      <c r="U16" s="47"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="54"/>
     </row>
     <row r="17" spans="1:21" ht="17" thickBot="1">
       <c r="A17" s="4"/>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="43"/>
-      <c r="L17" s="43"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="43"/>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="43"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="44"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="39"/>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="1"/>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="40" t="str">
-        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t ",$B18,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
-        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t Join.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
-      </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="40"/>
-      <c r="T18" s="40"/>
-      <c r="U18" s="41"/>
+      <c r="C18" s="49" t="str">
+        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t ",$B18,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
+        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t Join.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
+      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="50"/>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="1"/>
       <c r="B19" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="32" t="str">
-        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t ",$B19,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
-        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t Buy.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
-      </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="33"/>
+      <c r="C19" s="51" t="str">
+        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t ",$B19,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
+        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t Buy.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
+      </c>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="52"/>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="1"/>
       <c r="B20" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="32" t="str">
-        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t ",$B20,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
-        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t Send.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
-      </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="33"/>
+      <c r="C20" s="51" t="str">
+        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t ",$B20,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
+        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t Send.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
+      </c>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="52"/>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="1"/>
       <c r="B21" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="32" t="str">
-        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t ",$B21,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
-        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t Burn.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
-      </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="33"/>
+      <c r="C21" s="51" t="str">
+        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t ",$B21,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jthreads=",$C$7," -Jtps=",$B$13)</f>
+        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t Burn.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jthreads=8 -Jtps=3000</v>
+      </c>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="52"/>
     </row>
     <row r="22" spans="1:21" ht="17" thickBot="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="35" t="str">
-        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t ",$B22,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jloops_send=",$E$6," -Jthreads=",$C$7," -Jthreads_send=",$E$7," -Jtps=",$B$13)</f>
-        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -t Mix.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jloops_send=518400 -Jthreads=8 -Jthreads_send=50 -Jtps=3000</v>
-      </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="36"/>
+      <c r="C22" s="55" t="str">
+        <f>_xlfn.CONCAT("JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t ",$B22,".jmx -j meter.log -Jip=",$C$2," -Jport=",$C$3," -Jloops=",$C$6," -Jloops_send=",$E$6," -Jthreads=",$C$7," -Jthreads_send=",$E$7," -Jtps=",$B$13)</f>
+        <v>JVM_ARGS='-Xms2048m -Xmx2048m' jmeter -n -t Mix.jmx -j meter.log -Jip=192.168.1.1 -Jport=8080 -Jloops=33000 -Jloops_send=518400 -Jthreads=8 -Jthreads_send=50 -Jtps=3000</v>
+      </c>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="56"/>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="1"/>
@@ -1623,17 +1623,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C22:U22"/>
+    <mergeCell ref="C18:U18"/>
+    <mergeCell ref="C19:U19"/>
+    <mergeCell ref="C20:U20"/>
+    <mergeCell ref="C21:U21"/>
+    <mergeCell ref="C16:U16"/>
     <mergeCell ref="B17:U17"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C18:U18"/>
-    <mergeCell ref="C19:U19"/>
-    <mergeCell ref="C20:U20"/>
-    <mergeCell ref="C21:U21"/>
-    <mergeCell ref="C16:U16"/>
-    <mergeCell ref="C22:U22"/>
   </mergeCells>
   <conditionalFormatting sqref="C8">
     <cfRule type="expression" dxfId="1" priority="1">

</xml_diff>